<commit_message>
added feature specs for products index admin
</commit_message>
<xml_diff>
--- a/spec/fixtures/product_import_no_price.xlsx
+++ b/spec/fixtures/product_import_no_price.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>product_tags</t>
   </si>
@@ -30,12 +30,6 @@
     <t>vendors</t>
   </si>
   <si>
-    <t>category_collection</t>
-  </si>
-  <si>
-    <t>category_type</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
@@ -45,12 +39,6 @@
     <t>image</t>
   </si>
   <si>
-    <t>category_brand</t>
-  </si>
-  <si>
-    <t>sub_category</t>
-  </si>
-  <si>
     <t>Lightbulb Photo Holder</t>
   </si>
   <si>
@@ -69,9 +57,6 @@
     <t>Natural Reclaimed Wood</t>
   </si>
   <si>
-    <t>Organizer &amp; Display</t>
-  </si>
-  <si>
     <t>Hey, I've got an idea! How about you display that photo of you and your family/loved one/dog proudly and stylishly with these Lightbulb Photo Holders on an all natural reclaimed wood base? You'd rather just put a business card in there? A reminder note? A treasured Pokemon card? Who said photo holders aren't versatile!</t>
   </si>
   <si>
@@ -142,6 +127,33 @@
   </si>
   <si>
     <t>Worldwide</t>
+  </si>
+  <si>
+    <t>taxonomy_a</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>taxon_a</t>
+  </si>
+  <si>
+    <t>taxonomy_b</t>
+  </si>
+  <si>
+    <t>Collection</t>
+  </si>
+  <si>
+    <t>taxon_b</t>
+  </si>
+  <si>
+    <t>taxonomy_c</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>taxon_c</t>
   </si>
 </sst>
 </file>
@@ -786,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="78" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="78" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -800,39 +812,36 @@
     <col min="5" max="5" width="30.1640625" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="8" max="8" width="24.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" customWidth="1"/>
-    <col min="13" max="13" width="20.5" customWidth="1"/>
-    <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="15" max="15" width="25.1640625" customWidth="1"/>
-    <col min="16" max="16" width="25.1640625" style="1" customWidth="1"/>
-    <col min="19" max="22" width="14.5" style="1"/>
-    <col min="24" max="24" width="31" customWidth="1"/>
-    <col min="25" max="26" width="22.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="17" customWidth="1"/>
-    <col min="28" max="28" width="17" style="1" customWidth="1"/>
+    <col min="9" max="14" width="24.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" customWidth="1"/>
+    <col min="16" max="16" width="17" customWidth="1"/>
+    <col min="17" max="17" width="25.1640625" customWidth="1"/>
+    <col min="18" max="18" width="25.1640625" style="1" customWidth="1"/>
+    <col min="21" max="24" width="14.5" style="1"/>
+    <col min="26" max="26" width="31" customWidth="1"/>
+    <col min="27" max="28" width="22.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="17" customWidth="1"/>
+    <col min="30" max="30" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" customHeight="1">
+    <row r="1" spans="1:31" ht="15" customHeight="1">
       <c r="A1" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>2</v>
@@ -841,135 +850,146 @@
         <v>0</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="J1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="V1" s="13" t="s">
+      <c r="Z1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC1" s="13" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="2" spans="1:31" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="11">
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="11">
         <v>39</v>
       </c>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11" t="s">
-        <v>40</v>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>